<commit_message>
Updated Convenção de Nomenclatura
</commit_message>
<xml_diff>
--- a/bddad/Convenção de Nomenclatura.xlsx
+++ b/bddad/Convenção de Nomenclatura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpedr\OneDrive\Ambiente de Trabalho\BDDAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64B7A7D-1C85-4DAC-B91F-ECB51E3B2F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD52E26-4E77-4FAE-8F0C-9FF5D6181FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{BF63FABB-1833-4D5A-BEC1-3094D3094C57}"/>
+    <workbookView xWindow="-1095" yWindow="3300" windowWidth="21600" windowHeight="11505" xr2:uid="{BF63FABB-1833-4D5A-BEC1-3094D3094C57}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -325,16 +325,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>608814</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1595</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>15239</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1059180</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>164969</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>89297</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -349,8 +349,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7942082" y="427662"/>
-          <a:ext cx="4307500" cy="10487792"/>
+          <a:off x="7758517" y="443864"/>
+          <a:ext cx="4215122" cy="11504058"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -699,6 +699,37 @@
           <a:r>
             <a:rPr lang="pt-PT" sz="1100" b="0" i="0" u="none" baseline="0"/>
             <a:t>active_orders(_v)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="pt-PT" sz="1100" b="0" i="0" u="none" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" b="0" i="0" u="none" baseline="0"/>
+            <a:t>-&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1200" b="1" i="1" u="sng" baseline="0"/>
+            <a:t>Trigger</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" b="0" i="0" u="none" baseline="0"/>
+            <a:t>Deve ser atribuído o nome do objeto associado ao trigger, o objetivo do trigger, seguido do sufixo _trg</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" b="1" i="1" u="none" baseline="0"/>
+            <a:t>Exemplo:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="pt-PT" sz="1100" b="0" i="0" u="none" baseline="0"/>
+            <a:t>orders_journal_trg</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1007,28 +1038,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{502F097E-BB1A-431C-8767-EA54CE9464D5}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D47" zoomScale="194" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+    <sheetView tabSelected="1" topLeftCell="E45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" customWidth="1"/>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="8" max="8" width="15.109375" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1073,7 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1056,7 +1087,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1071,7 +1102,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1116,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1099,7 +1130,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1144,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1127,7 +1158,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -1141,7 +1172,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1155,7 +1186,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1169,7 +1200,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1183,7 +1214,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1197,7 +1228,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
@@ -1211,7 +1242,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>27</v>
       </c>
@@ -1225,7 +1256,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>28</v>
       </c>
@@ -1239,7 +1270,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -1253,7 +1284,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>32</v>
       </c>
@@ -1267,19 +1298,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>

</xml_diff>